<commit_message>
updated terms and privacy
</commit_message>
<xml_diff>
--- a/assets/dataFiles/Local Sightseeing (Hour Basis).xlsx
+++ b/assets/dataFiles/Local Sightseeing (Hour Basis).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bongu\Documents\TourNest-master\assets\dataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anjankumar.bnv\Documents\myproject\ootytaxi\assets\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE83AF-37F8-4DF8-BA70-FEF3201113BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72F45AD-5AA7-4E23-B472-B17DB7231CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="11" xr2:uid="{4D87A9C2-CEA1-4B8C-949D-4D16195EB809}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="7" xr2:uid="{4D87A9C2-CEA1-4B8C-949D-4D16195EB809}"/>
   </bookViews>
   <sheets>
     <sheet name="Local Sight Seeing (Hour Basis)" sheetId="1" r:id="rId1"/>
@@ -222,10 +222,6 @@
     <t>&lt;div&gt;&lt;h5&gt;You will visit&lt;/h5&gt;&lt;p&gt; Dodabetta Peak, Tea Factory &amp; Museum, Wax Museum, Chocolate Factory, Botanical Garden, Boathouse, Thread Garden, Ketty Valley view (view), MRC (outer view), Dolphin Nose, Lamb's Rock, Sim's Park, Tea Garden, Nigiris Mountain Toy Train. (9 hours)&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;h5&gt;You will visit&lt;/h5&gt;&lt;p&gt; Mudumalai Wild Life Sanctuary, Bison Valley View, Kalhatty Water Falls. 
-Falls (5 hours)&lt;/p&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;div&gt;&lt;h5&gt;You will visit&lt;/h5&gt;&lt;p&gt; Kateri Park, Black Thunder Wter Them Park, Law's Falls. (8 hours)&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
@@ -264,6 +260,9 @@
   </si>
   <si>
     <t>&lt;div&gt;&lt;h5&gt;You will visit&lt;/h5&gt;&lt;p&gt; Botanical Garden, Boathouse, Thread Garden, Century Rose Garden, Dodabetta Peak, Tea Factory, Pine Forest, 6th Mile (shooting spot), Kamarajar Sagar Dam,  9th Mile (shooting spot), Trible Village, Golf Course (outer view), Pykara falls, Pykara lake &amp; boating, Pykara Dam (outer view) (9 hours)&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;h5&gt;You will visit&lt;/h5&gt;&lt;p&gt;Mudumalai Wild Life Sanctuary, Bison Valley View, Kalhatty Water Falls.(5 hours)&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1109,7 @@
     </row>
     <row r="2" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1322,7 +1321,7 @@
     </row>
     <row r="2" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1506,7 +1505,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1534,7 +1533,7 @@
     </row>
     <row r="2" spans="1:7" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1949,7 +1948,7 @@
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -2154,7 +2153,7 @@
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -3188,8 +3187,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3216,7 +3215,7 @@
     </row>
     <row r="2" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -3428,7 +3427,7 @@
     </row>
     <row r="2" spans="1:7" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>

</xml_diff>